<commit_message>
build lambda and let into average_grad step by step
</commit_message>
<xml_diff>
--- a/fastai-excel/average_grad.xlsx
+++ b/fastai-excel/average_grad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Natsume/Documents/explore-fastai/fastai-excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97749A31-FE6E-934D-87FF-24E1971E3812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3AD1229-F5C6-E44B-A6E5-933903B4A82D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{9ADB88F8-8907-FF4F-B54E-37EA376C1290}"/>
   </bookViews>
@@ -25,7 +25,7 @@
     <definedName name="val">Sheet1!$A$2:$A$4</definedName>
     <definedName name="val_float">Sheet1!$A$7:$A$9</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -225,7 +225,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="83">
   <si>
     <t>ipdb&gt; a</t>
   </si>
@@ -320,9 +320,6 @@
     <t>grad_avg</t>
   </si>
   <si>
-    <t>None</t>
-  </si>
-  <si>
     <t>state</t>
   </si>
   <si>
@@ -2256,9 +2253,6 @@
     <t>p</t>
   </si>
   <si>
-    <t>p.grad.data</t>
-  </si>
-  <si>
     <t>Inputs or parameters</t>
   </si>
   <si>
@@ -2269,6 +2263,39 @@
   </si>
   <si>
     <t>lambda(p.grad.data, mom, dampening, grad_avg, let(ini_grad, if(grad_avg="None", RandArray(Rows(p.grad.data), Columns(p.grad.data),,,,False)*0, grad_avg), damp, if(dampening=FALSE, 1.0, 1-mom), p.grad.data*mom+grad_avg*damp))</t>
+  </si>
+  <si>
+    <t>average_grad</t>
+  </si>
+  <si>
+    <t>LAMBDA(p.grad.data,mom,dampening,grad_avg,A97#)</t>
+  </si>
+  <si>
+    <t>average_grad_1</t>
+  </si>
+  <si>
+    <t>average_grad_2</t>
+  </si>
+  <si>
+    <t>p.grad</t>
+  </si>
+  <si>
+    <t>LAMBDA(p,m,d,g,s,</t>
+  </si>
+  <si>
+    <t>IF(g=FALSE,p*m,p*0)) (B37#,A42,B42,C42,D42:D44)</t>
+  </si>
+  <si>
+    <t>lambda</t>
+  </si>
+  <si>
+    <t>average_grad_3</t>
+  </si>
+  <si>
+    <t>average_grad_4</t>
+  </si>
+  <si>
+    <t>create a droplist</t>
   </si>
 </sst>
 </file>
@@ -2726,16 +2753,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EDC3F99-ABC3-004C-9DF8-C1EA3E3832D1}">
   <dimension ref="A1:G108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.33203125" customWidth="1"/>
     <col min="2" max="2" width="16.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" customWidth="1"/>
     <col min="6" max="6" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2825,12 +2853,12 @@
         <v>6</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="G10" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="19" x14ac:dyDescent="0.25">
@@ -2841,7 +2869,7 @@
         <v>18</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="19" x14ac:dyDescent="0.25">
@@ -2854,7 +2882,7 @@
         <v>4</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="19" x14ac:dyDescent="0.25">
@@ -2865,7 +2893,7 @@
         <v>5</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="19" x14ac:dyDescent="0.25">
@@ -2876,27 +2904,27 @@
         <v>6</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="G15" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="7:7" ht="19" x14ac:dyDescent="0.25">
       <c r="G17" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="7:7" ht="19" x14ac:dyDescent="0.25">
       <c r="G18" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="7:7" ht="19" x14ac:dyDescent="0.25">
       <c r="G19" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="7:7" ht="19" x14ac:dyDescent="0.25">
@@ -2906,7 +2934,7 @@
     </row>
     <row r="21" spans="7:7" ht="19" x14ac:dyDescent="0.25">
       <c r="G21" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="7:7" ht="19" x14ac:dyDescent="0.25">
@@ -2916,7 +2944,7 @@
     </row>
     <row r="23" spans="7:7" ht="19" x14ac:dyDescent="0.25">
       <c r="G23" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="7:7" ht="19" x14ac:dyDescent="0.25">
@@ -2926,37 +2954,37 @@
     </row>
     <row r="25" spans="7:7" ht="19" x14ac:dyDescent="0.25">
       <c r="G25" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="7:7" ht="19" x14ac:dyDescent="0.25">
       <c r="G26" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="7:7" ht="19" x14ac:dyDescent="0.25">
       <c r="G27" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="7:7" ht="19" x14ac:dyDescent="0.25">
       <c r="G28" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="7:7" ht="19" x14ac:dyDescent="0.25">
       <c r="G29" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="7:7" ht="19" x14ac:dyDescent="0.25">
       <c r="G30" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="7:7" ht="19" x14ac:dyDescent="0.25">
       <c r="G31" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="19" x14ac:dyDescent="0.25">
@@ -2971,7 +2999,7 @@
     </row>
     <row r="35" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>2</v>
@@ -2979,10 +3007,10 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B36" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -3002,6 +3030,9 @@
       <c r="B38" s="2">
         <v>5</v>
       </c>
+      <c r="G38" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
@@ -3011,6 +3042,11 @@
         <v>6</v>
       </c>
     </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D40" t="s">
+        <v>82</v>
+      </c>
+    </row>
     <row r="41" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>28</v>
@@ -3022,10 +3058,13 @@
         <v>30</v>
       </c>
       <c r="D41" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="E41" t="s">
+        <v>72</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="19" x14ac:dyDescent="0.25">
@@ -3033,41 +3072,53 @@
         <v>0.9</v>
       </c>
       <c r="B42" t="b">
-        <v>0</v>
-      </c>
-      <c r="C42" t="s">
-        <v>31</v>
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>0.39999999999999991</v>
+      </c>
+      <c r="E42" t="s">
+        <v>77</v>
       </c>
       <c r="F42" s="2"/>
       <c r="G42" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="D43">
+        <v>0.49999999999999989</v>
+      </c>
+      <c r="E43" t="s">
+        <v>78</v>
+      </c>
       <c r="F43" s="2"/>
       <c r="G43" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="D44">
+        <v>0.59999999999999987</v>
+      </c>
       <c r="F44" s="2"/>
       <c r="G44" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="G45" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="G46" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="G47" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="19" x14ac:dyDescent="0.25">
@@ -3096,6 +3147,12 @@
       </c>
     </row>
     <row r="54" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>79</v>
+      </c>
+      <c r="D54" t="s">
+        <v>79</v>
+      </c>
       <c r="G54" s="1" t="s">
         <v>23</v>
       </c>
@@ -3104,6 +3161,12 @@
       <c r="A55" t="s">
         <v>30</v>
       </c>
+      <c r="C55" t="s">
+        <v>74</v>
+      </c>
+      <c r="D55" t="s">
+        <v>75</v>
+      </c>
       <c r="G55" s="1" t="s">
         <v>26</v>
       </c>
@@ -3111,7 +3174,17 @@
     <row r="56" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A56" cm="1">
         <f t="array" aca="1" ref="A56:A58" ca="1">IF(C42="None",_xlfn.RANDARRAY(ROWS(p.grad.data),1,,,FALSE)*0, D42:D44)</f>
+        <v>0.39999999999999991</v>
+      </c>
+      <c r="C56" cm="1">
+        <f t="array" ref="C56:C58">_xlfn.LAMBDA(_xlpm.p,_xlpm.m,_xlpm.d,_xlpm.g,
+IF(_xlpm.d=FALSE, _xlpm.p*_xlpm.m, _xlpm.p*0)
+)(_xlfn.ANCHORARRAY(B37),A42,B42,C42)</f>
         <v>0</v>
+      </c>
+      <c r="D56" s="2" cm="1">
+        <f t="array" ref="D56:D58">_xlfn.LAMBDA(_xlpm.p,_xlpm.m,_xlpm.d,_xlpm.g,_xlpm.s, IF(_xlpm.g="None",_xlpm.p*0,_xlpm.s))(_xlfn.ANCHORARRAY(B37),A42,B42,C42,D42:D44)</f>
+        <v>0.39999999999999991</v>
       </c>
       <c r="G56" s="1" t="s">
         <v>27</v>
@@ -3120,7 +3193,13 @@
     <row r="57" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A57">
         <f ca="1"/>
+        <v>0.49999999999999989</v>
+      </c>
+      <c r="C57">
         <v>0</v>
+      </c>
+      <c r="D57" s="2">
+        <v>0.49999999999999989</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>25</v>
@@ -3129,40 +3208,46 @@
     <row r="58" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A58">
         <f ca="1"/>
+        <v>0.59999999999999987</v>
+      </c>
+      <c r="C58">
         <v>0</v>
       </c>
+      <c r="D58" s="2">
+        <v>0.59999999999999987</v>
+      </c>
       <c r="G58" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="G59" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="G60" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="G61" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="G62" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="G63" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="G64" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="19" x14ac:dyDescent="0.25">
@@ -3187,60 +3272,76 @@
     </row>
     <row r="70" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="G70" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
+        <v>79</v>
+      </c>
       <c r="G71" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="C72" t="s">
+        <v>80</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <f>IF(B42=TRUE, 1-A42, 1)</f>
-        <v>1</v>
+        <v>9.9999999999999978E-2</v>
+      </c>
+      <c r="C73" s="2" cm="1">
+        <f t="array" ref="C73:C75">_xlfn.LAMBDA(_xlpm.p,_xlpm.m,_xlpm.d,_xlpm.g,_xlpm.s, _xlfn.LET(_xlpm.damp, IF(_xlpm.d=TRUE,1-_xlpm.m,1),IF(_xlpm.g="None",_xlpm.p*0,_xlpm.s)))(_xlfn.ANCHORARRAY(B37),A42,B42,C42,D42:D44)</f>
+        <v>0.39999999999999991</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
+      <c r="C74" s="2">
+        <v>0.49999999999999989</v>
+      </c>
       <c r="G74" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="C75" s="2">
+        <v>0.59999999999999987</v>
+      </c>
       <c r="G75" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="G76" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="G77" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="G78" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="G79" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="19" x14ac:dyDescent="0.25">
@@ -3270,7 +3371,7 @@
     </row>
     <row r="86" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="G86" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="19" x14ac:dyDescent="0.25">
@@ -3296,7 +3397,7 @@
     </row>
     <row r="92" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="G92" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="19" x14ac:dyDescent="0.25">
@@ -3308,52 +3409,68 @@
       <c r="G94" s="1"/>
     </row>
     <row r="95" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="C95" t="s">
+        <v>79</v>
+      </c>
       <c r="G95" s="1"/>
     </row>
     <row r="96" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>30</v>
       </c>
+      <c r="C96" t="s">
+        <v>81</v>
+      </c>
       <c r="G96" s="1"/>
     </row>
     <row r="97" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A97" s="2" cm="1">
         <f t="array" aca="1" ref="A97:A99" ca="1">_xlfn.ANCHORARRAY(A56)*A42+_xlfn.ANCHORARRAY(B37)*A73</f>
-        <v>4</v>
+        <v>0.75999999999999979</v>
+      </c>
+      <c r="C97" s="2" cm="1">
+        <f t="array" ref="C97:C99">_xlfn.LAMBDA(_xlpm.p,_xlpm.m,_xlpm.d,_xlpm.g,_xlpm.s, _xlfn.LET(_xlpm.damp, IF(_xlpm.d=TRUE,1-_xlpm.m,1), _xlpm.grad, IF(_xlpm.g="None",_xlpm.p*0,_xlpm.s), _xlpm.grad*_xlpm.m+_xlpm.p*_xlpm.damp))(_xlfn.ANCHORARRAY(B37),A42,B42,C42,D42:D44)</f>
+        <v>0.75999999999999979</v>
       </c>
       <c r="G97" s="1"/>
     </row>
     <row r="98" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <f ca="1"/>
-        <v>5</v>
+        <v>0.94999999999999973</v>
+      </c>
+      <c r="C98" s="2">
+        <v>0.94999999999999973</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="99" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <f ca="1"/>
-        <v>6</v>
+        <v>1.1399999999999997</v>
+      </c>
+      <c r="C99" s="2">
+        <v>1.1399999999999997</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
average_grad lambda is properly built
</commit_message>
<xml_diff>
--- a/fastai-excel/average_grad.xlsx
+++ b/fastai-excel/average_grad.xlsx
@@ -1,29 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10708"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Natsume/Documents/explore-fastai/fastai-excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3AD1229-F5C6-E44B-A6E5-933903B4A82D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71DFA015-D454-9F4C-BBA0-B9A6E6487284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{9ADB88F8-8907-FF4F-B54E-37EA376C1290}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <definedNames>
-    <definedName name="grad">Sheet1!$B$2:$B$4</definedName>
-    <definedName name="grad_avg_ini">Sheet1!$A$72:$A$74</definedName>
-    <definedName name="grad_float">Sheet1!$B$7:$B$9</definedName>
-    <definedName name="init_grad">Sheet1!$F$42:$F$44</definedName>
-    <definedName name="p">Sheet1!$A$12:$A$14</definedName>
-    <definedName name="p.grad.data">Sheet1!$B$12:$B$14</definedName>
-    <definedName name="val">Sheet1!$A$2:$A$4</definedName>
-    <definedName name="val_float">Sheet1!$A$7:$A$9</definedName>
+    <definedName name="average_grad">_xlfn.LAMBDA(_xlpm.p,_xlpm.m,_xlpm.d,_xlpm.g,_xlpm.s, _xlfn.LET(_xlpm.damp, IF(_xlpm.d=TRUE,1-_xlpm.m,1), _xlpm.grad, IF(_xlpm.g="None",_xlpm.p*0,_xlpm.s), _xlpm.grad*_xlpm.m+_xlpm.p*_xlpm.damp))</definedName>
+    <definedName name="grad_ini">Sheet1!$D$48:$D$51</definedName>
+    <definedName name="last_grad">Sheet1!$C$103:$C$106</definedName>
+    <definedName name="p.grad">Sheet1!$B$43:$B$46</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,10 +46,10 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>LiaoCan</author>
+    <author>DanielLC</author>
   </authors>
   <commentList>
-    <comment ref="B41" authorId="0" shapeId="0" xr:uid="{4C620D52-7A4D-B64B-BEBE-D8E6E9D35197}">
+    <comment ref="B42" authorId="0" shapeId="0" xr:uid="{9A43E1F5-7295-0C4D-B0C6-2A8BEB52C1BF}">
       <text>
         <r>
           <rPr>
@@ -60,7 +59,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>LiaoCan:</t>
+          <t>DanielLC:</t>
         </r>
         <r>
           <rPr>
@@ -79,11 +78,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>It can either be TRUE or FALSE</t>
+          <t>When having a different length of array, just change both the size of p.grad and last_grad and grad_ini in the Name Manager</t>
         </r>
       </text>
     </comment>
-    <comment ref="C41" authorId="0" shapeId="0" xr:uid="{70285541-E619-C442-84BC-C09CEE7D0C57}">
+    <comment ref="B47" authorId="0" shapeId="0" xr:uid="{DDB40617-CC25-FF47-9D14-1F63554B49B8}">
       <text>
         <r>
           <rPr>
@@ -93,7 +92,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>LiaoCan:</t>
+          <t>DanielLC:</t>
         </r>
         <r>
           <rPr>
@@ -112,12 +111,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">It can either be None or copy values from state from its right
-</t>
+          <t>Check below for true or false option</t>
         </r>
       </text>
     </comment>
-    <comment ref="D41" authorId="0" shapeId="0" xr:uid="{8DB2ECB6-1CF9-4344-8838-C19B7F939DF1}">
+    <comment ref="C47" authorId="0" shapeId="0" xr:uid="{1979C275-E29E-474C-93C2-227DA1258B81}">
       <text>
         <r>
           <rPr>
@@ -127,7 +125,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>LiaoCan:</t>
+          <t>DanielLC:</t>
         </r>
         <r>
           <rPr>
@@ -146,40 +144,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>It receives the output grad_avg from the bottom</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A96" authorId="0" shapeId="0" xr:uid="{AC10B71D-7E9C-9045-86F1-178D939BCC91}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>LiaoCan:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">you should copy this output into state </t>
+          <t>Click the cell below to select an option</t>
         </r>
       </text>
     </comment>
@@ -189,9 +154,8 @@
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="2">
+  <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
@@ -202,30 +166,16 @@
       </extLst>
     </bk>
   </futureMetadata>
-  <futureMetadata name="XLRICHVALUE" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
   <cellMetadata count="1">
     <bk>
       <rc t="1" v="0"/>
     </bk>
   </cellMetadata>
-  <valueMetadata count="1">
-    <bk>
-      <rc t="2" v="0"/>
-    </bk>
-  </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="80">
   <si>
     <t>ipdb&gt; a</t>
   </si>
@@ -2256,18 +2206,6 @@
     <t>Inputs or parameters</t>
   </si>
   <si>
-    <t>average_grad will save grad_avg into state, so copy it into state, and then copy it from state to grad_avg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lambda(p.grad.data, mom, dampening, grad_avg, let(ini_grad, if(grad_avg="None", RandArray(Rows(p.grad.data), Columns(p.grad.data),,,,False)*0, grad_avg), damp, if(dampening=FALSE, 1.0, 1-mom), p.grad.data*mom+grad_avg*damp)) </t>
-  </si>
-  <si>
-    <t>lambda(p.grad.data, mom, dampening, grad_avg, let(ini_grad, if(grad_avg="None", RandArray(Rows(p.grad.data), Columns(p.grad.data),,,,False)*0, grad_avg), damp, if(dampening=FALSE, 1.0, 1-mom), p.grad.data*mom+grad_avg*damp))</t>
-  </si>
-  <si>
-    <t>average_grad</t>
-  </si>
-  <si>
     <t>LAMBDA(p.grad.data,mom,dampening,grad_avg,A97#)</t>
   </si>
   <si>
@@ -2280,12 +2218,6 @@
     <t>p.grad</t>
   </si>
   <si>
-    <t>LAMBDA(p,m,d,g,s,</t>
-  </si>
-  <si>
-    <t>IF(g=FALSE,p*m,p*0)) (B37#,A42,B42,C42,D42:D44)</t>
-  </si>
-  <si>
     <t>lambda</t>
   </si>
   <si>
@@ -2295,14 +2227,23 @@
     <t>average_grad_4</t>
   </si>
   <si>
-    <t>create a droplist</t>
+    <t>Implementing tst_param</t>
+  </si>
+  <si>
+    <t>Implementing average_grad</t>
+  </si>
+  <si>
+    <t>Check State</t>
+  </si>
+  <si>
+    <t>Make it real</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2353,16 +2294,46 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -2370,15 +2341,151 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color theme="9"/>
+      </left>
+      <right style="double">
+        <color theme="9"/>
+      </right>
+      <top style="double">
+        <color theme="9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color theme="9"/>
+      </left>
+      <right style="double">
+        <color theme="9"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color theme="9"/>
+      </left>
+      <right style="double">
+        <color theme="9"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color theme="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="5" tint="0.59996337778862885"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color theme="5" tint="0.59996337778862885"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color theme="5" tint="0.59996337778862885"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color theme="5" tint="0.59996337778862885"/>
+      </right>
+      <top style="thick">
+        <color theme="5" tint="0.59996337778862885"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="5" tint="0.59996337778862885"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color theme="5" tint="0.59996337778862885"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="5" tint="0.59996337778862885"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="5" tint="0.59996337778862885"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="5" tint="0.59996337778862885"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color theme="5" tint="0.59996337778862885"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="5" tint="0.59996337778862885"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2396,62 +2503,110 @@
 </styleSheet>
 </file>
 
-<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
-<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
-  <global>
-    <keyFlags>
-      <key name="_Self">
-        <flag name="ExcludeFromFile" value="1"/>
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_DisplayString">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Flags">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Format">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_SubLabel">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Attribution">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Icon">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_Display">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_CanonicalPropertyNames">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-      <key name="_ClassificationId">
-        <flag name="ExcludeFromCalcComparison" value="1"/>
-      </key>
-    </keyFlags>
-  </global>
-</rvTypesInfo>
+<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
 </file>
 
-<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
-  <rv s="0">
-    <v>13</v>
-    <v>7</v>
-  </rv>
-</rvData>
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>88900</xdr:colOff>
+          <xdr:row>45</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>1104900</xdr:colOff>
+          <xdr:row>46</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1033" name="Button 9" descr="copy" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1033"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{341B3804-A844-6582-5828-0F1F8B488F86}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
+                  <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+                </a:rPr>
+                <a:t>copy from last</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri" pitchFamily="2" charset="0"/>
+                <a:cs typeface="Calibri" pitchFamily="2" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData fPrintsWithSheet="0"/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
 </file>
 
-<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
-<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
-  <s t="_error">
-    <k n="errorType" t="i"/>
-    <k n="subType" t="i"/>
-  </s>
-</rvStructures>
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <definedNames>
+      <definedName name="Macro1"/>
+    </definedNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2751,736 +2906,845 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EDC3F99-ABC3-004C-9DF8-C1EA3E3832D1}">
-  <dimension ref="A1:G108"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:G111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="1" max="1" width="24.5" customWidth="1"/>
     <col min="2" max="2" width="16.83203125" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="19.33203125" customWidth="1"/>
     <col min="6" max="6" width="17.6640625" customWidth="1"/>
+    <col min="7" max="7" width="126.1640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>14</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G2" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B3" s="1">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G3" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B4" s="1">
         <v>5</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G4" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B5" s="1">
         <v>6</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G5" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G5" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G6" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>16</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G7" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" cm="1">
-        <f t="array" ref="A7:A9">ROUND(val, 2)</f>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="G10" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G11" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="G13" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="G14" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="G15" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G16" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" spans="7:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G18" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="7:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G19" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="7:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G20" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="7:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G21" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="7:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G22" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="7:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G23" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="7:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G24" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="7:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G25" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="7:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G26" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="7:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G27" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="7:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G28" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="7:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G29" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="7:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G30" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="7:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G31" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="7:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G32" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G33" s="4"/>
+    </row>
+    <row r="34" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G34" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G35" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="2" cm="1">
-        <f t="array" ref="B7:B9">ROUND(grad,2)*1</f>
+    </row>
+    <row r="36" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G36" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G37" s="4"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G38" s="4"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G39" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G40" s="4"/>
+    </row>
+    <row r="41" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="G41" s="4"/>
+    </row>
+    <row r="42" spans="1:7" ht="20" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C42" s="12"/>
+      <c r="D42" s="13"/>
+      <c r="G42" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A43" s="14" cm="1">
+        <f t="array" ref="A43:A45">A3:A5</f>
+        <v>1</v>
+      </c>
+      <c r="B43" s="9" cm="1">
+        <f t="array" ref="B43:B45">B3:B5</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
+      <c r="C43" s="2"/>
+      <c r="D43" s="15"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A44" s="14">
         <v>2</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B44" s="9">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="C44" s="2"/>
+      <c r="D44" s="15"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A45" s="14">
         <v>3</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B45" s="9">
         <v>6</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G10" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" cm="1">
-        <f t="array" ref="A12:A14">val_float</f>
+      <c r="C45" s="2"/>
+      <c r="D45" s="15"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A46" s="16"/>
+      <c r="B46" s="9">
+        <v>7</v>
+      </c>
+      <c r="C46" s="2"/>
+      <c r="D46" s="15"/>
+      <c r="G46" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A47" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D47" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E47" s="20"/>
+      <c r="G47" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A48" s="16">
+        <v>0.9</v>
+      </c>
+      <c r="B48" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B12" s="2" cm="1">
-        <f t="array" ref="B12:B14">grad_float</f>
-        <v>4</v>
-      </c>
-      <c r="G12" s="3" t="s">
+      <c r="C48" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D48" s="21">
+        <v>0.39999999999999991</v>
+      </c>
+      <c r="G48" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" s="16"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="21">
+        <v>0.49999999999999989</v>
+      </c>
+      <c r="G49" s="4"/>
+    </row>
+    <row r="50" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A50" s="16"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="21">
+        <v>0.59999999999999987</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A51" s="16"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="22">
+        <v>0.69999999999999984</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A52" s="16"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="15"/>
+      <c r="G52" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A53" s="16"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="15"/>
+      <c r="G53" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A54" s="16"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="15"/>
+      <c r="G54" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A55" s="16"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="15"/>
+      <c r="G55" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="17"/>
+      <c r="B56" s="18"/>
+      <c r="C56" s="18"/>
+      <c r="D56" s="19"/>
+      <c r="G56" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="20" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="G57" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G58" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G59" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>73</v>
+      </c>
+      <c r="D60" t="s">
+        <v>73</v>
+      </c>
+      <c r="G60" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>30</v>
+      </c>
+      <c r="C61" t="s">
+        <v>70</v>
+      </c>
+      <c r="D61" t="s">
+        <v>71</v>
+      </c>
+      <c r="G61" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>2</v>
-      </c>
-      <c r="B13" s="2">
-        <v>5</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>3</v>
-      </c>
-      <c r="B14" s="2">
-        <v>6</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G15" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="7:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G17" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="7:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G18" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="7:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G19" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="7:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G20" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="7:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G21" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="7:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G22" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="7:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G23" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="7:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G24" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="7:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G25" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="7:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G26" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="7:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G27" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="28" spans="7:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G28" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="29" spans="7:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G29" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="30" spans="7:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G30" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="31" spans="7:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G31" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G33" s="1" t="s">
+    <row r="62" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A62" cm="1">
+        <f t="array" aca="1" ref="A62:A64" ca="1">IF(C48="None",_xlfn.RANDARRAY(ROWS(p.grad),1,,,FALSE)*0, D48:D50)</f>
+        <v>0.39999999999999991</v>
+      </c>
+      <c r="C62" cm="1">
+        <f t="array" ref="C62:C65">_xlfn.LAMBDA(_xlpm.p,_xlpm.m,_xlpm.d,_xlpm.g,
+IF(_xlpm.d=FALSE, _xlpm.p*_xlpm.m, _xlpm.p*0)
+)(p.grad,A48,B48,C48)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G34" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>68</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>67</v>
-      </c>
-      <c r="B36" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" cm="1">
-        <f t="array" ref="A37:A39">p</f>
-        <v>1</v>
-      </c>
-      <c r="B37" s="2" cm="1">
-        <f t="array" ref="B37:B39">p.grad.data</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="2">
-        <v>2</v>
-      </c>
-      <c r="B38" s="2">
-        <v>5</v>
-      </c>
-      <c r="G38" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="2">
-        <v>3</v>
-      </c>
-      <c r="B39" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D40" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>28</v>
-      </c>
-      <c r="B41" t="s">
-        <v>29</v>
-      </c>
-      <c r="C41" t="s">
-        <v>30</v>
-      </c>
-      <c r="D41" t="s">
-        <v>31</v>
-      </c>
-      <c r="E41" t="s">
-        <v>72</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>0.9</v>
-      </c>
-      <c r="B42" t="b">
-        <v>1</v>
-      </c>
-      <c r="D42">
+      <c r="D62" s="1" cm="1">
+        <f t="array" ref="D62:D65">_xlfn.LAMBDA(_xlpm.p,_xlpm.m,_xlpm.d,_xlpm.g,_xlpm.s, IF(_xlpm.g="None",_xlpm.p*0,_xlpm.s))(p.grad,A48,B48,C48,grad_ini)</f>
         <v>0.39999999999999991</v>
       </c>
-      <c r="E42" t="s">
-        <v>77</v>
-      </c>
-      <c r="F42" s="2"/>
-      <c r="G42" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="D43">
-        <v>0.49999999999999989</v>
-      </c>
-      <c r="E43" t="s">
-        <v>78</v>
-      </c>
-      <c r="F43" s="2"/>
-      <c r="G43" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="D44">
-        <v>0.59999999999999987</v>
-      </c>
-      <c r="F44" s="2"/>
-      <c r="G44" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G45" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G46" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G47" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G49" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G50" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G51" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G52" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G53" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="C54" t="s">
-        <v>79</v>
-      </c>
-      <c r="D54" t="s">
-        <v>79</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>30</v>
-      </c>
-      <c r="C55" t="s">
-        <v>74</v>
-      </c>
-      <c r="D55" t="s">
-        <v>75</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A56" cm="1">
-        <f t="array" aca="1" ref="A56:A58" ca="1">IF(C42="None",_xlfn.RANDARRAY(ROWS(p.grad.data),1,,,FALSE)*0, D42:D44)</f>
-        <v>0.39999999999999991</v>
-      </c>
-      <c r="C56" cm="1">
-        <f t="array" ref="C56:C58">_xlfn.LAMBDA(_xlpm.p,_xlpm.m,_xlpm.d,_xlpm.g,
-IF(_xlpm.d=FALSE, _xlpm.p*_xlpm.m, _xlpm.p*0)
-)(_xlfn.ANCHORARRAY(B37),A42,B42,C42)</f>
-        <v>0</v>
-      </c>
-      <c r="D56" s="2" cm="1">
-        <f t="array" ref="D56:D58">_xlfn.LAMBDA(_xlpm.p,_xlpm.m,_xlpm.d,_xlpm.g,_xlpm.s, IF(_xlpm.g="None",_xlpm.p*0,_xlpm.s))(_xlfn.ANCHORARRAY(B37),A42,B42,C42,D42:D44)</f>
-        <v>0.39999999999999991</v>
-      </c>
-      <c r="G56" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A57">
+      <c r="G62" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A63">
         <f ca="1"/>
         <v>0.49999999999999989</v>
       </c>
-      <c r="C57">
+      <c r="C63">
         <v>0</v>
       </c>
-      <c r="D57" s="2">
+      <c r="D63" s="1">
         <v>0.49999999999999989</v>
       </c>
-      <c r="G57" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A58">
+      <c r="G63" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A64">
         <f ca="1"/>
         <v>0.59999999999999987</v>
       </c>
-      <c r="C58">
+      <c r="C64">
         <v>0</v>
       </c>
-      <c r="D58" s="2">
+      <c r="D64" s="1">
         <v>0.59999999999999987</v>
       </c>
-      <c r="G58" s="1" t="s">
+      <c r="G64" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>0.69999999999999984</v>
+      </c>
+      <c r="G65" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G66" s="4"/>
+    </row>
+    <row r="67" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G67" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G68" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G69" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G70" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G71" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G72" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G73" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G74" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G75" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G59" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G60" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G61" s="3" t="s">
+    <row r="76" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G76" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="C77" t="s">
+        <v>73</v>
+      </c>
+      <c r="G77" s="6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G62" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G63" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G64" s="3" t="s">
+    <row r="78" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C78" t="s">
+        <v>74</v>
+      </c>
+      <c r="G78" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <f>IF(B48=TRUE, 1-A48, 1)</f>
+        <v>9.9999999999999978E-2</v>
+      </c>
+      <c r="C79" s="1" cm="1">
+        <f t="array" ref="C79:C82">_xlfn.LAMBDA(_xlpm.p,_xlpm.m,_xlpm.d,_xlpm.g,_xlpm.s, _xlfn.LET(_xlpm.damp, IF(_xlpm.d=TRUE,1-_xlpm.m,1),IF(_xlpm.g="None",_xlpm.p*0,_xlpm.s)))(p.grad,A48,B48,C48,grad_ini)</f>
+        <v>0.39999999999999991</v>
+      </c>
+      <c r="G79" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A80" s="1"/>
+      <c r="C80" s="1">
+        <v>0.49999999999999989</v>
+      </c>
+      <c r="G80" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G66" s="1" t="s">
+    <row r="81" spans="3:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="C81" s="1">
+        <v>0.59999999999999987</v>
+      </c>
+      <c r="G81" s="6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="82" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C82">
+        <v>0.69999999999999984</v>
+      </c>
+      <c r="G82" s="4"/>
+    </row>
+    <row r="83" spans="3:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G83" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G67" s="1" t="s">
+    <row r="84" spans="3:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G84" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G68" s="1" t="s">
+    <row r="85" spans="3:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G85" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G69" s="1" t="s">
+    <row r="86" spans="3:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G86" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G70" s="1" t="s">
+    <row r="87" spans="3:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G87" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="C71" t="s">
-        <v>79</v>
-      </c>
-      <c r="G71" s="1" t="s">
+    <row r="88" spans="3:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G88" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C72" t="s">
-        <v>80</v>
-      </c>
-      <c r="G72" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A73" s="2">
-        <f>IF(B42=TRUE, 1-A42, 1)</f>
-        <v>9.9999999999999978E-2</v>
-      </c>
-      <c r="C73" s="2" cm="1">
-        <f t="array" ref="C73:C75">_xlfn.LAMBDA(_xlpm.p,_xlpm.m,_xlpm.d,_xlpm.g,_xlpm.s, _xlfn.LET(_xlpm.damp, IF(_xlpm.d=TRUE,1-_xlpm.m,1),IF(_xlpm.g="None",_xlpm.p*0,_xlpm.s)))(_xlfn.ANCHORARRAY(B37),A42,B42,C42,D42:D44)</f>
-        <v>0.39999999999999991</v>
-      </c>
-      <c r="G73" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A74" s="2"/>
-      <c r="C74" s="2">
-        <v>0.49999999999999989</v>
-      </c>
-      <c r="G74" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="C75" s="2">
-        <v>0.59999999999999987</v>
-      </c>
-      <c r="G75" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G76" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G77" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G78" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G79" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G80" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G82" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G83" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G84" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G85" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G86" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G87" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G88" s="1"/>
-    </row>
-    <row r="89" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G89" s="1"/>
-    </row>
-    <row r="90" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G90" s="1" t="s">
+    <row r="89" spans="3:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G89" s="5"/>
+    </row>
+    <row r="90" spans="3:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G90" s="5"/>
+    </row>
+    <row r="91" spans="3:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G91" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G91" s="1" t="s">
+    <row r="92" spans="3:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G92" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G92" s="1" t="s">
+    <row r="93" spans="3:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G93" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G93" s="1">
+    <row r="94" spans="3:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G94" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="G94" s="1"/>
-    </row>
-    <row r="95" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="C95" t="s">
-        <v>79</v>
-      </c>
-      <c r="G95" s="1"/>
-    </row>
-    <row r="96" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+    <row r="95" spans="3:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G95" s="5"/>
+    </row>
+    <row r="96" spans="3:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G96" s="5"/>
+    </row>
+    <row r="97" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G97" s="5"/>
+    </row>
+    <row r="98" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G98" s="5"/>
+    </row>
+    <row r="99" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G99" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="G100" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C101" t="s">
+        <v>73</v>
+      </c>
+      <c r="G101" s="4"/>
+    </row>
+    <row r="102" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>30</v>
       </c>
-      <c r="C96" t="s">
-        <v>81</v>
-      </c>
-      <c r="G96" s="1"/>
-    </row>
-    <row r="97" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A97" s="2" cm="1">
-        <f t="array" aca="1" ref="A97:A99" ca="1">_xlfn.ANCHORARRAY(A56)*A42+_xlfn.ANCHORARRAY(B37)*A73</f>
+      <c r="C102" t="s">
+        <v>75</v>
+      </c>
+      <c r="G102" s="7"/>
+    </row>
+    <row r="103" spans="1:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A103" s="1" cm="1">
+        <f t="array" aca="1" ref="A103:A105" ca="1">_xlfn.ANCHORARRAY(A62)*A48+_xlfn.ANCHORARRAY(B43)*A79</f>
         <v>0.75999999999999979</v>
       </c>
-      <c r="C97" s="2" cm="1">
-        <f t="array" ref="C97:C99">_xlfn.LAMBDA(_xlpm.p,_xlpm.m,_xlpm.d,_xlpm.g,_xlpm.s, _xlfn.LET(_xlpm.damp, IF(_xlpm.d=TRUE,1-_xlpm.m,1), _xlpm.grad, IF(_xlpm.g="None",_xlpm.p*0,_xlpm.s), _xlpm.grad*_xlpm.m+_xlpm.p*_xlpm.damp))(_xlfn.ANCHORARRAY(B37),A42,B42,C42,D42:D44)</f>
+      <c r="C103" s="1" cm="1">
+        <f t="array" ref="C103:C106">_xlfn.LAMBDA(_xlpm.p,_xlpm.m,_xlpm.d,_xlpm.g,_xlpm.s, _xlfn.LET(_xlpm.damp, IF(_xlpm.d=TRUE,1-_xlpm.m,1), _xlpm.grad, IF(_xlpm.g="None",_xlpm.p*0,_xlpm.s), _xlpm.grad*_xlpm.m+_xlpm.p*_xlpm.damp))(p.grad,A48,B48,C48,grad_ini)</f>
         <v>0.75999999999999979</v>
       </c>
-      <c r="G97" s="1"/>
-    </row>
-    <row r="98" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A98" s="2">
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A104" s="1">
         <f ca="1"/>
         <v>0.94999999999999973</v>
       </c>
-      <c r="C98" s="2">
+      <c r="C104" s="1">
         <v>0.94999999999999973</v>
       </c>
-      <c r="G98" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="A99" s="2">
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A105" s="1">
         <f ca="1"/>
         <v>1.1399999999999997</v>
       </c>
-      <c r="C99" s="2">
+      <c r="C105" s="1">
         <v>1.1399999999999997</v>
       </c>
-      <c r="G99" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A101" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A105" t="s">
-        <v>70</v>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C106" s="1">
+        <v>1.3299999999999996</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A107" t="s">
-        <v>71</v>
+      <c r="C107" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A108" t="e" cm="1" vm="1">
-        <f t="array" ref="A108">_xlfn.LAMBDA(_xlpm.a,_xlpm.b, _xlpm.a+_xlpm.b)</f>
-        <v>#VALUE!</v>
+      <c r="C108" s="1" cm="1">
+        <f t="array" ref="C108:C111">average_grad(p.grad,A48,B48,C48,grad_ini)</f>
+        <v>0.75999999999999979</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C109" s="1">
+        <v>0.94999999999999973</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C110" s="1">
+        <v>1.1399999999999997</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C111" s="1">
+        <v>1.3299999999999996</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C48" xr:uid="{384B88E2-ED2B-E145-B60D-341A93ABCF0B}">
+      <formula1>"None, Check State"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B48" xr:uid="{AE4AD949-C312-1549-822D-8D313579D6E2}">
+      <formula1>"TRUE,FALSE"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1033" r:id="rId3" name="Button 9">
+              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[1]!Macro1" altText="copy">
+                <anchor moveWithCells="1" sizeWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>88900</xdr:colOff>
+                    <xdr:row>45</xdr:row>
+                    <xdr:rowOff>38100</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>1104900</xdr:colOff>
+                    <xdr:row>46</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
average_grad and momentum_step Lambda done
</commit_message>
<xml_diff>
--- a/fastai-excel/average_grad.xlsx
+++ b/fastai-excel/average_grad.xlsx
@@ -8,21 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Natsume/Documents/explore-fastai/fastai-excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71DFA015-D454-9F4C-BBA0-B9A6E6487284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A76818-2A58-844F-A4B6-85181B3FB49A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{9ADB88F8-8907-FF4F-B54E-37EA376C1290}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="1" xr2:uid="{9ADB88F8-8907-FF4F-B54E-37EA376C1290}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="average_grad" sheetId="1" r:id="rId1"/>
+    <sheet name="momentum_step" sheetId="2" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId2"/>
+    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
+    <definedName name="average_grad" localSheetId="1">_xlfn.LAMBDA(_xlpm.p,_xlpm.m,_xlpm.d,_xlpm.g,_xlpm.s, _xlfn.LET(_xlpm.damp, IF(_xlpm.d=TRUE,1-_xlpm.m,1), _xlpm.grad, IF(_xlpm.g="None",_xlpm.p*0,_xlpm.s), _xlpm.grad*_xlpm.m+_xlpm.p*_xlpm.damp))</definedName>
     <definedName name="average_grad">_xlfn.LAMBDA(_xlpm.p,_xlpm.m,_xlpm.d,_xlpm.g,_xlpm.s, _xlfn.LET(_xlpm.damp, IF(_xlpm.d=TRUE,1-_xlpm.m,1), _xlpm.grad, IF(_xlpm.g="None",_xlpm.p*0,_xlpm.s), _xlpm.grad*_xlpm.m+_xlpm.p*_xlpm.damp))</definedName>
-    <definedName name="grad_ini">Sheet1!$D$48:$D$51</definedName>
-    <definedName name="last_grad">Sheet1!$C$103:$C$106</definedName>
-    <definedName name="p.grad">Sheet1!$B$43:$B$46</definedName>
+    <definedName name="grad_ini" localSheetId="1">#REF!</definedName>
+    <definedName name="grad_ini">average_grad!$D$48:$D$51</definedName>
+    <definedName name="last_grad" localSheetId="1">#REF!</definedName>
+    <definedName name="last_grad">average_grad!$C$103:$C$106</definedName>
+    <definedName name="momentum_step">_xlfn.LAMBDA(_xlpm.p_data,_xlpm.lr,_xlpm.grad, _xlpm.p_data-_xlpm.lr*_xlpm.grad)</definedName>
+    <definedName name="p.grad" localSheetId="1">#REF!</definedName>
+    <definedName name="p.grad">average_grad!$B$43:$B$46</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -152,6 +159,115 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>DanielLC</author>
+  </authors>
+  <commentList>
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{DA9F3ABA-11EB-6D4D-A36F-63A8830DD30F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>DanielLC:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>When having a different length of array, just change both the size of p.grad and last_grad and grad_ini in the Name Manager</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{5CDA6E25-9398-9C4D-BF7C-010D49FCBE8F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>DanielLC:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Check below for true or false option</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{2C2717DF-9DF9-B24B-8FBB-F1364E8C1D41}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>DanielLC:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Click the cell below to select an option</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
@@ -175,7 +291,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="89">
   <si>
     <t>ipdb&gt; a</t>
   </si>
@@ -2237,6 +2353,33 @@
   </si>
   <si>
     <t>Make it real</t>
+  </si>
+  <si>
+    <t>momentum_step</t>
+  </si>
+  <si>
+    <t>named lambda</t>
+  </si>
+  <si>
+    <t>lambda without a name</t>
+  </si>
+  <si>
+    <t>average_grad</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>lr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    p.data.add_(grad_avg, alpha=-lr)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "Step for SGD with momentum with `lr`"</t>
+  </si>
+  <si>
+    <t>def momentum_step(p, lr, grad_avg, **kwargs):</t>
   </si>
 </sst>
 </file>
@@ -2303,6 +2446,7 @@
     </font>
     <font>
       <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -2532,7 +2676,7 @@
                   <a14:compatExt spid="_x0000_s1033"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{341B3804-A844-6582-5828-0F1F8B488F86}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2606,6 +2750,12 @@
       <sheetData sheetId="0"/>
     </sheetDataSet>
   </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </externalLink>
 </file>
 
@@ -2909,7 +3059,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+    <sheetView topLeftCell="A29" workbookViewId="0">
       <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
@@ -3747,4 +3897,234 @@
     </mc:Choice>
   </mc:AlternateContent>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80D82EAE-325B-F647-A9D6-A7ABF759103B}">
+  <dimension ref="A1:L27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" s="13"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="14">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>1E-3</v>
+      </c>
+      <c r="D7" s="15"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="14">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1">
+        <v>5</v>
+      </c>
+      <c r="D8" s="15"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="14">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1">
+        <v>6</v>
+      </c>
+      <c r="D9" s="15"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="16">
+        <v>4</v>
+      </c>
+      <c r="B10" s="1">
+        <v>7</v>
+      </c>
+      <c r="D10" s="15"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="16">
+        <v>0.9</v>
+      </c>
+      <c r="B12" t="b">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12" s="21">
+        <v>0.39999999999999991</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="16"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="21">
+        <v>0.49999999999999989</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" s="16"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="21">
+        <v>0.59999999999999987</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="16"/>
+      <c r="D15" s="22">
+        <v>0.69999999999999984</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" cm="1">
+        <f t="array" ref="A17:A20">average_grad(B7:B10,A12,B12,C12,D12:D15)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>82</v>
+      </c>
+      <c r="C22" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>80</v>
+      </c>
+      <c r="C23" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" cm="1">
+        <f t="array" ref="A24:A27">_xlfn.LAMBDA(_xlpm.p_data,_xlpm.lr,_xlpm.grad, _xlpm.p_data-_xlpm.lr*_xlpm.grad)(A7:A10,C7,_xlfn.ANCHORARRAY(A17))</f>
+        <v>0.996</v>
+      </c>
+      <c r="C24" cm="1">
+        <f t="array" ref="C24:C27">momentum_step(A7:A10,C7,_xlfn.ANCHORARRAY(A17))</f>
+        <v>0.996</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>1.9950000000000001</v>
+      </c>
+      <c r="C25">
+        <v>1.9950000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>2.9940000000000002</v>
+      </c>
+      <c r="C26">
+        <v>2.9940000000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>3.9929999999999999</v>
+      </c>
+      <c r="C27">
+        <v>3.9929999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12" xr:uid="{ED0D9DB8-3B96-CA40-A897-A213788E3B10}">
+      <formula1>"None, Check State"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12" xr:uid="{4E9AF067-E559-0345-BA68-6ED6DB7DE893}">
+      <formula1>"TRUE,FALSE"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>